<commit_message>
Add totals to parser and averager. Add to excel data about school.
</commit_message>
<xml_diff>
--- a/data-parser/SchoolExpenses.xlsx
+++ b/data-parser/SchoolExpenses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="0" windowWidth="17580" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18040" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="296">
   <si>
     <t>Clyde Miller Academy</t>
   </si>
@@ -289,6 +289,624 @@
   </si>
   <si>
     <t>Therapeutic School Alternative</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>1000 No. Grand, 63106</t>
+  </si>
+  <si>
+    <t>(314) 371-0394</t>
+  </si>
+  <si>
+    <t>Jana Haywood</t>
+  </si>
+  <si>
+    <t>5101 McRee, 63110</t>
+  </si>
+  <si>
+    <t>(314) 776-3300</t>
+  </si>
+  <si>
+    <t>Amy Phillips</t>
+  </si>
+  <si>
+    <t>4915 Donovan Ave, 63109</t>
+  </si>
+  <si>
+    <t>(314) 481-4095</t>
+  </si>
+  <si>
+    <t>Kimberly Long</t>
+  </si>
+  <si>
+    <t>4939 Kemper Ave, 63139</t>
+  </si>
+  <si>
+    <t>(314) 776-1301</t>
+  </si>
+  <si>
+    <t>Victoria Shearing</t>
+  </si>
+  <si>
+    <t>4041 S. Broadway, 63118</t>
+  </si>
+  <si>
+    <t>(314)456-0582</t>
+  </si>
+  <si>
+    <t>Jonathan Griffin</t>
+  </si>
+  <si>
+    <t>1547 S. Theresa Avenue, 63104</t>
+  </si>
+  <si>
+    <t>(314) 696-2290</t>
+  </si>
+  <si>
+    <t>Frederick Steele</t>
+  </si>
+  <si>
+    <t>5140 Riverview Blvd, 63120</t>
+  </si>
+  <si>
+    <t>(314) 385-4774</t>
+  </si>
+  <si>
+    <t>Chris Crumble</t>
+  </si>
+  <si>
+    <t>4015 McPherson, 63108</t>
+  </si>
+  <si>
+    <t>(314) 534-3894</t>
+  </si>
+  <si>
+    <t>Steven Lawler</t>
+  </si>
+  <si>
+    <t>2156 Russell, 63104</t>
+  </si>
+  <si>
+    <t>(314) 773-0027</t>
+  </si>
+  <si>
+    <t>Nakia King</t>
+  </si>
+  <si>
+    <t>3230 Hartford Avenue, 63118</t>
+  </si>
+  <si>
+    <t>(314) 776-6040</t>
+  </si>
+  <si>
+    <t>Enna Dancy</t>
+  </si>
+  <si>
+    <t>918 No. Union, 63108</t>
+  </si>
+  <si>
+    <t>(314) 367-9222</t>
+  </si>
+  <si>
+    <t>Thomas Cason</t>
+  </si>
+  <si>
+    <t>4268 W. Cottage Ave., 63113</t>
+  </si>
+  <si>
+    <t>(314) 371-1048</t>
+  </si>
+  <si>
+    <t>Sean Nichols</t>
+  </si>
+  <si>
+    <t>3035 Cass Ave., 63106</t>
+  </si>
+  <si>
+    <t>(314) 533-9487</t>
+  </si>
+  <si>
+    <t>Brenda M. Smith</t>
+  </si>
+  <si>
+    <t>3125 S. Kingshighway, 63139</t>
+  </si>
+  <si>
+    <t>(314) 771-2772</t>
+  </si>
+  <si>
+    <t>Kacy Seals</t>
+  </si>
+  <si>
+    <t>4265 Athlone Ave., 63115</t>
+  </si>
+  <si>
+    <t>(314) 261-8131</t>
+  </si>
+  <si>
+    <t>Chip Clatto</t>
+  </si>
+  <si>
+    <t>5910 Clifton, 63109</t>
+  </si>
+  <si>
+    <t>(314) 352-1043</t>
+  </si>
+  <si>
+    <t>Robert Lescher</t>
+  </si>
+  <si>
+    <t>1004 No Jefferson, 63106</t>
+  </si>
+  <si>
+    <t>(314) 231-0413</t>
+  </si>
+  <si>
+    <t>Darwin Young</t>
+  </si>
+  <si>
+    <t>3417 Grace Ave., 63116</t>
+  </si>
+  <si>
+    <t>(314) 772-1038</t>
+  </si>
+  <si>
+    <t>Lisa Brown</t>
+  </si>
+  <si>
+    <t>1200 N. Jefferson, 63106</t>
+  </si>
+  <si>
+    <t>(314) 241-2295</t>
+  </si>
+  <si>
+    <t>A. Michael Shaw</t>
+  </si>
+  <si>
+    <t>3021 Hickory St., 63104</t>
+  </si>
+  <si>
+    <t>(314) 932-1464</t>
+  </si>
+  <si>
+    <t>CeAndre Perry</t>
+  </si>
+  <si>
+    <t>5028 Morganford Road, 63116</t>
+  </si>
+  <si>
+    <t>(314) 481-3440</t>
+  </si>
+  <si>
+    <t>Benicia Nanex-Hunt</t>
+  </si>
+  <si>
+    <t>5130 Oakland, 63110</t>
+  </si>
+  <si>
+    <t>(314) 652-9282</t>
+  </si>
+  <si>
+    <t>Susan Reid</t>
+  </si>
+  <si>
+    <t>1311 Tower Grove Ave, 63110</t>
+  </si>
+  <si>
+    <t>(314) 535-3910</t>
+  </si>
+  <si>
+    <t>Felicia Miller</t>
+  </si>
+  <si>
+    <t>3921 No. Newstead, 63115</t>
+  </si>
+  <si>
+    <t>(314) 385-4767</t>
+  </si>
+  <si>
+    <t>Paula Brodie</t>
+  </si>
+  <si>
+    <t>2128 Gano, 63107</t>
+  </si>
+  <si>
+    <t>(314) 534-0370</t>
+  </si>
+  <si>
+    <t>Sarah Briscoe</t>
+  </si>
+  <si>
+    <t>5319 Lansdowne Ave., 63109</t>
+  </si>
+  <si>
+    <t>(314) 352-4343</t>
+  </si>
+  <si>
+    <t>Anna Russell</t>
+  </si>
+  <si>
+    <t>3325 Bell Avenue, 63106</t>
+  </si>
+  <si>
+    <t>(314) 345-5690</t>
+  </si>
+  <si>
+    <t>Brandon Clay</t>
+  </si>
+  <si>
+    <t>2900 Hadley, 63107</t>
+  </si>
+  <si>
+    <t>(314) 241-7165</t>
+  </si>
+  <si>
+    <t>JaVeeta Parks-Prince</t>
+  </si>
+  <si>
+    <t>3820 No. 14th St., 63107</t>
+  </si>
+  <si>
+    <t>(314) 231-9608</t>
+  </si>
+  <si>
+    <t>Tierrus Nance</t>
+  </si>
+  <si>
+    <t>3120 St. Louis Ave., 63106</t>
+  </si>
+  <si>
+    <t>(314) 533-2750</t>
+  </si>
+  <si>
+    <t>DeSonda Payton</t>
+  </si>
+  <si>
+    <t>6746 Clayton, 63139</t>
+  </si>
+  <si>
+    <t>(319) 645-4845</t>
+  </si>
+  <si>
+    <t>Andrew Donovan</t>
+  </si>
+  <si>
+    <t>1415 No. Garrison Ave., 63106</t>
+  </si>
+  <si>
+    <t>(314) 533-2526</t>
+  </si>
+  <si>
+    <t>Anthony Virdure</t>
+  </si>
+  <si>
+    <t>4025 Sullivan Ave., 63107</t>
+  </si>
+  <si>
+    <t>(314) 531-1198</t>
+  </si>
+  <si>
+    <t>Patricia Cox</t>
+  </si>
+  <si>
+    <t>1383 Clara Ave., 63112</t>
+  </si>
+  <si>
+    <t>(314) 383-0836</t>
+  </si>
+  <si>
+    <t>Michelle McDaniel</t>
+  </si>
+  <si>
+    <t>3709 Nebraska Ave., 63118</t>
+  </si>
+  <si>
+    <t>(314) 771-3533</t>
+  </si>
+  <si>
+    <t>Jim Triplett</t>
+  </si>
+  <si>
+    <t>#4 Gateway Dr., 63106</t>
+  </si>
+  <si>
+    <t>(314) 241-8255</t>
+  </si>
+  <si>
+    <t>Karen Austin-Lindsey</t>
+  </si>
+  <si>
+    <t>#2 Gateway Dr., 63106</t>
+  </si>
+  <si>
+    <t>(314) 241-0993</t>
+  </si>
+  <si>
+    <t>5819 Westminster Place, 63112</t>
+  </si>
+  <si>
+    <t>(314) 367-0552</t>
+  </si>
+  <si>
+    <t>Starlett Frenchie</t>
+  </si>
+  <si>
+    <t>1220 N. 10th Street, 63112</t>
+  </si>
+  <si>
+    <t>(314) 231-7284</t>
+  </si>
+  <si>
+    <t>Deborah Rogers</t>
+  </si>
+  <si>
+    <t>5831 Pamplin Place, 63147</t>
+  </si>
+  <si>
+    <t>(314) 385-2212</t>
+  </si>
+  <si>
+    <t>Oluyemisi Folarin</t>
+  </si>
+  <si>
+    <t>3111 Cora Ave., 63115</t>
+  </si>
+  <si>
+    <t>(314) 383-2550</t>
+  </si>
+  <si>
+    <t>Deandria Wallace</t>
+  </si>
+  <si>
+    <t>1616 California, 63104</t>
+  </si>
+  <si>
+    <t>(314) 771-2539</t>
+  </si>
+  <si>
+    <t>Julia Kaiser</t>
+  </si>
+  <si>
+    <t>2516 S. 9th Street, 63104</t>
+  </si>
+  <si>
+    <t>(314) 932-5720</t>
+  </si>
+  <si>
+    <t>Jacqueline Russell</t>
+  </si>
+  <si>
+    <t>1301 Hogan St., 63106</t>
+  </si>
+  <si>
+    <t>(314) 231-2459</t>
+  </si>
+  <si>
+    <t>Leslie Bonner</t>
+  </si>
+  <si>
+    <t>5031 Potomac, 63139</t>
+  </si>
+  <si>
+    <t>(314) 353-8875</t>
+  </si>
+  <si>
+    <t>Steven Kyle Jefferson</t>
+  </si>
+  <si>
+    <t>5821 Kennerly Ave., 63112</t>
+  </si>
+  <si>
+    <t>(314) 385-0546</t>
+  </si>
+  <si>
+    <t>DaMaris White</t>
+  </si>
+  <si>
+    <t>5030 Lexington Ave., 63115</t>
+  </si>
+  <si>
+    <t>(314) 385-2522</t>
+  </si>
+  <si>
+    <t>Angelique Brown</t>
+  </si>
+  <si>
+    <t>516 Loughborough, 63111</t>
+  </si>
+  <si>
+    <t>(314) 353-1349</t>
+  </si>
+  <si>
+    <t>Ingrid Iskali</t>
+  </si>
+  <si>
+    <t>6020 Pernod, 63139</t>
+  </si>
+  <si>
+    <t>(314) 352-9212</t>
+  </si>
+  <si>
+    <t>Cicely Johnson</t>
+  </si>
+  <si>
+    <t>4047 Juniata St., 63116</t>
+  </si>
+  <si>
+    <t>(314) 772-4545</t>
+  </si>
+  <si>
+    <t>Angela Glass</t>
+  </si>
+  <si>
+    <t>6031 Southwest Ave., 63139</t>
+  </si>
+  <si>
+    <t>(314) 645-1201</t>
+  </si>
+  <si>
+    <t>Deborah Leto</t>
+  </si>
+  <si>
+    <t>2745 Meramec St., 63118</t>
+  </si>
+  <si>
+    <t>(314) 353-7145</t>
+  </si>
+  <si>
+    <t>Jonathan Strong</t>
+  </si>
+  <si>
+    <t>3641 Missouri Ave., 63118</t>
+  </si>
+  <si>
+    <t>(314) 776-7315</t>
+  </si>
+  <si>
+    <t>Sonya Wayne</t>
+  </si>
+  <si>
+    <t>4221 Shaw Blvd., 63110</t>
+  </si>
+  <si>
+    <t>(314) 772-0994</t>
+  </si>
+  <si>
+    <t>Kelli Casper</t>
+  </si>
+  <si>
+    <t>8959 Riverview Blvd., 63147</t>
+  </si>
+  <si>
+    <t>(314) 867-0634</t>
+  </si>
+  <si>
+    <t>Natasha Mitchell</t>
+  </si>
+  <si>
+    <t>1530 S. Grand, 63104</t>
+  </si>
+  <si>
+    <t>(314) 776-3285</t>
+  </si>
+  <si>
+    <t>Nicole Conaway</t>
+  </si>
+  <si>
+    <t>4300 Morganford Rd., 63116</t>
+  </si>
+  <si>
+    <t>(314) 481-0420</t>
+  </si>
+  <si>
+    <t>Tina Hamilton</t>
+  </si>
+  <si>
+    <t>3935 Enright, 63108</t>
+  </si>
+  <si>
+    <t>(314) 533-0894</t>
+  </si>
+  <si>
+    <t>Angel Nave</t>
+  </si>
+  <si>
+    <t>1224 S. 14th St., 63104</t>
+  </si>
+  <si>
+    <t>(314) 241-1533</t>
+  </si>
+  <si>
+    <t>Shaimeka Humphrey</t>
+  </si>
+  <si>
+    <t>5329 Columbia, 63139</t>
+  </si>
+  <si>
+    <t>(314) 776-5091</t>
+  </si>
+  <si>
+    <t>Lori Craig</t>
+  </si>
+  <si>
+    <t>3412 Shenandoah Ave., 63014</t>
+  </si>
+  <si>
+    <t>(314) 772-7544</t>
+  </si>
+  <si>
+    <t>Chad Rooney</t>
+  </si>
+  <si>
+    <t>2050 Allen Ave., 63014</t>
+  </si>
+  <si>
+    <t>(314) 771-0010</t>
+  </si>
+  <si>
+    <t>Hollie Russell-West</t>
+  </si>
+  <si>
+    <t>647 Tower Grove, 63110</t>
+  </si>
+  <si>
+    <t>(314) 533-0874</t>
+  </si>
+  <si>
+    <t>Diane Dymond</t>
+  </si>
+  <si>
+    <t>5000 Davison Ave., 63120</t>
+  </si>
+  <si>
+    <t>(314) 383-1829</t>
+  </si>
+  <si>
+    <t>Mildred Moore</t>
+  </si>
+  <si>
+    <t>1130 No. Euclid, 63113</t>
+  </si>
+  <si>
+    <t>(314) 361-0432</t>
+  </si>
+  <si>
+    <t>Lisa Small</t>
+  </si>
+  <si>
+    <t>1921 Prather, 63139</t>
+  </si>
+  <si>
+    <t>(314) 645-1202</t>
+  </si>
+  <si>
+    <t>Yvette Levy</t>
+  </si>
+  <si>
+    <t>6131 Leona, 63116</t>
+  </si>
+  <si>
+    <t>(314) 481-8585</t>
+  </si>
+  <si>
+    <t>Margaret Meyer</t>
+  </si>
+  <si>
+    <t>725 Bellerive Blvd., 63111</t>
+  </si>
+  <si>
+    <t>(314) 353-1346</t>
+  </si>
+  <si>
+    <t>Carla Cunigan</t>
   </si>
 </sst>
 </file>
@@ -685,20 +1303,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S76"/>
+  <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="T69" sqref="T69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="28.83203125" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" customWidth="1"/>
+    <col min="22" max="22" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -756,8 +1378,17 @@
       <c r="S1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -815,8 +1446,17 @@
       <c r="S2">
         <v>135791</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -874,8 +1514,17 @@
       <c r="S3">
         <v>113723</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -933,8 +1582,17 @@
       <c r="S4">
         <v>35122</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" t="s">
+        <v>100</v>
+      </c>
+      <c r="V4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -992,8 +1650,17 @@
       <c r="S5">
         <v>21533</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5" t="s">
+        <v>102</v>
+      </c>
+      <c r="U5" t="s">
+        <v>103</v>
+      </c>
+      <c r="V5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1051,8 +1718,17 @@
       <c r="S6">
         <v>67092</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="T6" t="s">
+        <v>105</v>
+      </c>
+      <c r="U6" t="s">
+        <v>106</v>
+      </c>
+      <c r="V6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1110,8 +1786,17 @@
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="T7" t="s">
+        <v>108</v>
+      </c>
+      <c r="U7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1169,8 +1854,17 @@
       <c r="S8">
         <v>2167</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="T8" t="s">
+        <v>111</v>
+      </c>
+      <c r="U8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1204,8 +1898,17 @@
       <c r="K9">
         <v>129045</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="T9" t="s">
+        <v>114</v>
+      </c>
+      <c r="U9" t="s">
+        <v>115</v>
+      </c>
+      <c r="V9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1263,8 +1966,17 @@
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10" t="s">
+        <v>117</v>
+      </c>
+      <c r="U10" t="s">
+        <v>118</v>
+      </c>
+      <c r="V10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1322,8 +2034,17 @@
       <c r="S11">
         <v>65705</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11" t="s">
+        <v>120</v>
+      </c>
+      <c r="U11" t="s">
+        <v>121</v>
+      </c>
+      <c r="V11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1381,8 +2102,17 @@
       <c r="S12">
         <v>4961</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="T12" t="s">
+        <v>123</v>
+      </c>
+      <c r="U12" t="s">
+        <v>124</v>
+      </c>
+      <c r="V12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1440,8 +2170,17 @@
       <c r="S13">
         <v>31129</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="T13" t="s">
+        <v>126</v>
+      </c>
+      <c r="U13" t="s">
+        <v>127</v>
+      </c>
+      <c r="V13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1499,8 +2238,17 @@
       <c r="S14">
         <v>52770</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="T14" t="s">
+        <v>129</v>
+      </c>
+      <c r="U14" t="s">
+        <v>130</v>
+      </c>
+      <c r="V14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1558,8 +2306,17 @@
       <c r="S15">
         <v>37996</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="T15" t="s">
+        <v>132</v>
+      </c>
+      <c r="U15" t="s">
+        <v>133</v>
+      </c>
+      <c r="V15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1617,8 +2374,17 @@
       <c r="S16">
         <v>173</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="T16" t="s">
+        <v>135</v>
+      </c>
+      <c r="U16" t="s">
+        <v>136</v>
+      </c>
+      <c r="V16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1676,8 +2442,17 @@
       <c r="S17">
         <v>8034</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="T17" t="s">
+        <v>138</v>
+      </c>
+      <c r="U17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1735,8 +2510,17 @@
       <c r="S18">
         <v>11985</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="T18" t="s">
+        <v>141</v>
+      </c>
+      <c r="U18" t="s">
+        <v>142</v>
+      </c>
+      <c r="V18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1770,8 +2554,17 @@
       <c r="K19">
         <v>38893</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="T19" t="s">
+        <v>117</v>
+      </c>
+      <c r="U19" t="s">
+        <v>118</v>
+      </c>
+      <c r="V19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1829,8 +2622,17 @@
       <c r="S20">
         <v>184227</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="T20" t="s">
+        <v>144</v>
+      </c>
+      <c r="U20" t="s">
+        <v>145</v>
+      </c>
+      <c r="V20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1888,8 +2690,17 @@
       <c r="S21">
         <v>155327</v>
       </c>
-    </row>
-    <row r="22" spans="1:19">
+      <c r="T21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U21" t="s">
+        <v>148</v>
+      </c>
+      <c r="V21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1947,8 +2758,17 @@
       <c r="S22">
         <v>10059</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="T22" t="s">
+        <v>150</v>
+      </c>
+      <c r="U22" t="s">
+        <v>151</v>
+      </c>
+      <c r="V22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2006,8 +2826,17 @@
       <c r="S23">
         <v>565</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="T23" t="s">
+        <v>153</v>
+      </c>
+      <c r="U23" t="s">
+        <v>154</v>
+      </c>
+      <c r="V23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2065,8 +2894,17 @@
       <c r="S24">
         <v>22535</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="T24" t="s">
+        <v>156</v>
+      </c>
+      <c r="U24" t="s">
+        <v>157</v>
+      </c>
+      <c r="V24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2124,8 +2962,17 @@
       <c r="S25">
         <v>205245</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="T25" t="s">
+        <v>159</v>
+      </c>
+      <c r="U25" t="s">
+        <v>160</v>
+      </c>
+      <c r="V25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2183,8 +3030,17 @@
       <c r="S26">
         <v>396</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="T26" t="s">
+        <v>162</v>
+      </c>
+      <c r="U26" t="s">
+        <v>163</v>
+      </c>
+      <c r="V26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2242,8 +3098,17 @@
       <c r="S27">
         <v>4143</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="T27" t="s">
+        <v>165</v>
+      </c>
+      <c r="U27" t="s">
+        <v>166</v>
+      </c>
+      <c r="V27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2301,8 +3166,17 @@
       <c r="S28">
         <v>56654</v>
       </c>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="T28" t="s">
+        <v>168</v>
+      </c>
+      <c r="U28" t="s">
+        <v>169</v>
+      </c>
+      <c r="V28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2360,8 +3234,17 @@
       <c r="S29">
         <v>5201</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="T29" t="s">
+        <v>171</v>
+      </c>
+      <c r="U29" t="s">
+        <v>172</v>
+      </c>
+      <c r="V29" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2419,8 +3302,17 @@
       <c r="S30">
         <v>16334</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="T30" t="s">
+        <v>174</v>
+      </c>
+      <c r="U30" t="s">
+        <v>175</v>
+      </c>
+      <c r="V30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2478,8 +3370,17 @@
       <c r="S31">
         <v>427</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="T31" t="s">
+        <v>177</v>
+      </c>
+      <c r="U31" t="s">
+        <v>178</v>
+      </c>
+      <c r="V31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2537,8 +3438,17 @@
       <c r="S32">
         <v>571</v>
       </c>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="T32" t="s">
+        <v>180</v>
+      </c>
+      <c r="U32" t="s">
+        <v>181</v>
+      </c>
+      <c r="V32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2596,8 +3506,17 @@
       <c r="S33">
         <v>53816</v>
       </c>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="T33" t="s">
+        <v>183</v>
+      </c>
+      <c r="U33" t="s">
+        <v>184</v>
+      </c>
+      <c r="V33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2655,8 +3574,17 @@
       <c r="S34">
         <v>395</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34" t="s">
+        <v>186</v>
+      </c>
+      <c r="U34" t="s">
+        <v>187</v>
+      </c>
+      <c r="V34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -2714,8 +3642,17 @@
       <c r="S35">
         <v>263</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="T35" t="s">
+        <v>189</v>
+      </c>
+      <c r="U35" t="s">
+        <v>190</v>
+      </c>
+      <c r="V35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2773,8 +3710,17 @@
       <c r="S36">
         <v>148228</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="T36" t="s">
+        <v>192</v>
+      </c>
+      <c r="U36" t="s">
+        <v>193</v>
+      </c>
+      <c r="V36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2832,8 +3778,17 @@
       <c r="S37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="T37" t="s">
+        <v>195</v>
+      </c>
+      <c r="U37" t="s">
+        <v>196</v>
+      </c>
+      <c r="V37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -2891,8 +3846,17 @@
       <c r="S38">
         <v>34282</v>
       </c>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="T38" t="s">
+        <v>198</v>
+      </c>
+      <c r="U38" t="s">
+        <v>199</v>
+      </c>
+      <c r="V38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -2950,8 +3914,17 @@
       <c r="S39">
         <v>10001</v>
       </c>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="T39" t="s">
+        <v>201</v>
+      </c>
+      <c r="U39" t="s">
+        <v>202</v>
+      </c>
+      <c r="V39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -3009,8 +3982,17 @@
       <c r="S40">
         <v>59069</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40" t="s">
+        <v>203</v>
+      </c>
+      <c r="U40" t="s">
+        <v>204</v>
+      </c>
+      <c r="V40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -3068,8 +4050,17 @@
       <c r="S41">
         <v>18836</v>
       </c>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="T41" t="s">
+        <v>206</v>
+      </c>
+      <c r="U41" t="s">
+        <v>207</v>
+      </c>
+      <c r="V41" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3127,8 +4118,17 @@
       <c r="S42">
         <v>4730</v>
       </c>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="T42" t="s">
+        <v>209</v>
+      </c>
+      <c r="U42" t="s">
+        <v>210</v>
+      </c>
+      <c r="V42" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -3186,8 +4186,17 @@
       <c r="S43">
         <v>456</v>
       </c>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="T43" t="s">
+        <v>212</v>
+      </c>
+      <c r="U43" t="s">
+        <v>213</v>
+      </c>
+      <c r="V43" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -3245,8 +4254,17 @@
       <c r="S44">
         <v>708</v>
       </c>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="T44" t="s">
+        <v>215</v>
+      </c>
+      <c r="U44" t="s">
+        <v>216</v>
+      </c>
+      <c r="V44" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -3304,8 +4322,17 @@
       <c r="S45">
         <v>1367</v>
       </c>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="T45" t="s">
+        <v>218</v>
+      </c>
+      <c r="U45" t="s">
+        <v>219</v>
+      </c>
+      <c r="V45" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -3363,8 +4390,17 @@
       <c r="S46">
         <v>234987</v>
       </c>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="T46" t="s">
+        <v>221</v>
+      </c>
+      <c r="U46" t="s">
+        <v>222</v>
+      </c>
+      <c r="V46" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -3422,8 +4458,17 @@
       <c r="S47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="T47" t="s">
+        <v>224</v>
+      </c>
+      <c r="U47" t="s">
+        <v>225</v>
+      </c>
+      <c r="V47" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -3481,8 +4526,17 @@
       <c r="S48">
         <v>82</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="T48" t="s">
+        <v>227</v>
+      </c>
+      <c r="U48" t="s">
+        <v>228</v>
+      </c>
+      <c r="V48" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -3540,8 +4594,17 @@
       <c r="S49">
         <v>43009</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="T49" t="s">
+        <v>230</v>
+      </c>
+      <c r="U49" t="s">
+        <v>231</v>
+      </c>
+      <c r="V49" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -3599,8 +4662,17 @@
       <c r="S50">
         <v>922</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="T50" t="s">
+        <v>233</v>
+      </c>
+      <c r="U50" t="s">
+        <v>234</v>
+      </c>
+      <c r="V50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -3658,8 +4730,17 @@
       <c r="S51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="T51" t="s">
+        <v>236</v>
+      </c>
+      <c r="U51" t="s">
+        <v>237</v>
+      </c>
+      <c r="V51" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -3717,8 +4798,17 @@
       <c r="S52">
         <v>2804</v>
       </c>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="T52" t="s">
+        <v>239</v>
+      </c>
+      <c r="U52" t="s">
+        <v>240</v>
+      </c>
+      <c r="V52" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -3776,8 +4866,17 @@
       <c r="S53">
         <v>64617</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
+      <c r="T53" t="s">
+        <v>242</v>
+      </c>
+      <c r="U53" t="s">
+        <v>243</v>
+      </c>
+      <c r="V53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -3835,8 +4934,17 @@
       <c r="S54">
         <v>5546</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="T54" t="s">
+        <v>245</v>
+      </c>
+      <c r="U54" t="s">
+        <v>246</v>
+      </c>
+      <c r="V54" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -3894,8 +5002,17 @@
       <c r="S55">
         <v>133414</v>
       </c>
-    </row>
-    <row r="56" spans="1:19">
+      <c r="T55" t="s">
+        <v>248</v>
+      </c>
+      <c r="U55" t="s">
+        <v>249</v>
+      </c>
+      <c r="V55" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -3953,8 +5070,17 @@
       <c r="S56">
         <v>3677</v>
       </c>
-    </row>
-    <row r="57" spans="1:19">
+      <c r="T56" t="s">
+        <v>251</v>
+      </c>
+      <c r="U56" t="s">
+        <v>252</v>
+      </c>
+      <c r="V56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -4012,8 +5138,17 @@
       <c r="S57">
         <v>25150</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
+      <c r="T57" t="s">
+        <v>254</v>
+      </c>
+      <c r="U57" t="s">
+        <v>255</v>
+      </c>
+      <c r="V57" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -4071,8 +5206,17 @@
       <c r="S58">
         <v>44807</v>
       </c>
-    </row>
-    <row r="59" spans="1:19">
+      <c r="T58" t="s">
+        <v>257</v>
+      </c>
+      <c r="U58" t="s">
+        <v>258</v>
+      </c>
+      <c r="V58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -4130,8 +5274,17 @@
       <c r="S59">
         <v>1150</v>
       </c>
-    </row>
-    <row r="60" spans="1:19">
+      <c r="T59" t="s">
+        <v>260</v>
+      </c>
+      <c r="U59" t="s">
+        <v>261</v>
+      </c>
+      <c r="V59" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -4189,8 +5342,17 @@
       <c r="S60">
         <v>2750</v>
       </c>
-    </row>
-    <row r="61" spans="1:19">
+      <c r="T60" t="s">
+        <v>263</v>
+      </c>
+      <c r="U60" t="s">
+        <v>264</v>
+      </c>
+      <c r="V60" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -4248,8 +5410,17 @@
       <c r="S61">
         <v>310</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
+      <c r="T61" t="s">
+        <v>266</v>
+      </c>
+      <c r="U61" t="s">
+        <v>267</v>
+      </c>
+      <c r="V61" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -4307,8 +5478,17 @@
       <c r="S62">
         <v>9533</v>
       </c>
-    </row>
-    <row r="63" spans="1:19">
+      <c r="T62" t="s">
+        <v>269</v>
+      </c>
+      <c r="U62" t="s">
+        <v>270</v>
+      </c>
+      <c r="V62" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -4366,8 +5546,17 @@
       <c r="S63">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:19">
+      <c r="T63" t="s">
+        <v>272</v>
+      </c>
+      <c r="U63" t="s">
+        <v>273</v>
+      </c>
+      <c r="V63" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -4425,8 +5614,17 @@
       <c r="S64">
         <v>1933</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
+      <c r="T64" t="s">
+        <v>275</v>
+      </c>
+      <c r="U64" t="s">
+        <v>276</v>
+      </c>
+      <c r="V64" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -4484,8 +5682,17 @@
       <c r="S65">
         <v>28416</v>
       </c>
-    </row>
-    <row r="66" spans="1:19">
+      <c r="T65" t="s">
+        <v>278</v>
+      </c>
+      <c r="U65" t="s">
+        <v>279</v>
+      </c>
+      <c r="V65" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -4543,8 +5750,17 @@
       <c r="S66">
         <v>1934</v>
       </c>
-    </row>
-    <row r="67" spans="1:19">
+      <c r="T66" t="s">
+        <v>281</v>
+      </c>
+      <c r="U66" t="s">
+        <v>282</v>
+      </c>
+      <c r="V66" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -4602,8 +5818,17 @@
       <c r="S67">
         <v>1732</v>
       </c>
-    </row>
-    <row r="68" spans="1:19">
+      <c r="T67" t="s">
+        <v>284</v>
+      </c>
+      <c r="U67" t="s">
+        <v>285</v>
+      </c>
+      <c r="V67" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -4661,8 +5886,17 @@
       <c r="S68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
+      <c r="T68" t="s">
+        <v>287</v>
+      </c>
+      <c r="U68" t="s">
+        <v>288</v>
+      </c>
+      <c r="V68" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -4720,8 +5954,17 @@
       <c r="S69">
         <v>54420</v>
       </c>
-    </row>
-    <row r="70" spans="1:19">
+      <c r="T69" t="s">
+        <v>290</v>
+      </c>
+      <c r="U69" t="s">
+        <v>291</v>
+      </c>
+      <c r="V69" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -4779,8 +6022,17 @@
       <c r="S70">
         <v>20183</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
+      <c r="T70" t="s">
+        <v>293</v>
+      </c>
+      <c r="U70" t="s">
+        <v>294</v>
+      </c>
+      <c r="V70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -4839,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:22">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -4898,7 +6150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:22">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -4957,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:22">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -4992,7 +6244,7 @@
         <v>9211</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -5027,7 +6279,7 @@
         <v>7978</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:22">
       <c r="A76" t="s">
         <v>89</v>
       </c>

</xml_diff>